<commit_message>
Atualização do Relatório Mensal de Ordens de Serviços para Junho/2016.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201606.xlsx
+++ b/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201606.xlsx
@@ -17,7 +17,7 @@
     <sheet name="SLA" sheetId="2" r:id="rId3"/>
     <sheet name="Tipos de OS" sheetId="6" state="hidden" r:id="rId4"/>
     <sheet name="ControleOSsMês" sheetId="7" state="hidden" r:id="rId5"/>
-    <sheet name="Situação" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="Situação" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Mensal!$A$2:$AG$154</definedName>
@@ -1685,10 +1685,10 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,10 +1786,10 @@
         <v>4721</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="C2" s="52">
-        <v>42444</v>
+        <v>42520</v>
       </c>
       <c r="D2" t="s">
         <v>96</v>
@@ -1807,7 +1807,9 @@
       <c r="I2" s="52">
         <v>42444</v>
       </c>
-      <c r="J2" s="52"/>
+      <c r="J2" s="52">
+        <v>42520</v>
+      </c>
       <c r="K2" s="52"/>
       <c r="L2" s="52"/>
       <c r="M2" s="21">
@@ -1828,10 +1830,10 @@
         <v>4757</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="C3" s="52">
-        <v>42486</v>
+        <v>42500</v>
       </c>
       <c r="D3" t="s">
         <v>96</v>
@@ -1846,7 +1848,9 @@
         <v>42493</v>
       </c>
       <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
+      <c r="I3" s="52">
+        <v>42500</v>
+      </c>
       <c r="J3" s="52"/>
       <c r="K3" s="52"/>
       <c r="L3" s="52"/>
@@ -1868,10 +1872,10 @@
         <v>4776</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="52">
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="D4" t="s">
         <v>96</v>
@@ -1882,7 +1886,9 @@
       <c r="F4" s="52">
         <v>42514</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="52">
+        <v>42521</v>
+      </c>
       <c r="H4" s="52"/>
       <c r="I4" s="52"/>
       <c r="J4" s="52"/>
@@ -1906,10 +1912,10 @@
         <v>4777</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C5" s="52">
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
@@ -1920,14 +1926,16 @@
       <c r="F5" s="52">
         <v>42514</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="52">
+        <v>42521</v>
+      </c>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="52"/>
       <c r="L5" s="52"/>
       <c r="M5" s="21">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="N5" s="21"/>
       <c r="O5" s="71"/>
@@ -1959,7 +1967,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,7 +1997,7 @@
         <v>119</v>
       </c>
       <c r="B1" s="64">
-        <v>42495</v>
+        <v>42526</v>
       </c>
       <c r="D1" s="62"/>
       <c r="E1" s="65" t="s">
@@ -2144,7 +2152,7 @@
       </c>
       <c r="B5" s="73" t="str">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Plano Entregue</v>
+        <v>Entregue</v>
       </c>
       <c r="C5" s="73"/>
       <c r="D5" s="54" t="str">
@@ -2153,7 +2161,7 @@
       </c>
       <c r="E5" s="59">
         <f>IF(A5="","",VLOOKUP(A5,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42444</v>
+        <v>42520</v>
       </c>
       <c r="F5" s="56" t="str">
         <f>IF(A5="","","Titulo:")</f>
@@ -2225,12 +2233,12 @@
         <v>42515</v>
       </c>
       <c r="J6" s="20">
-        <f>IF(I6="","",WORKDAY(I6,IF(IF(P7="",P6,P7)&lt;150,5,10)))</f>
-        <v>42529</v>
+        <f>IF(I6="","",WORKDAY(IF(I7="",I6,I7),IF(IF(P7="",P6,P7)&lt;150,5,10)))</f>
+        <v>42534</v>
       </c>
       <c r="K6" s="20">
         <f>IF(J6="","",J6+ROUND((IF(P7="",P6,P7)/(19*LN(IF(P7="",P6,P7))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42554</v>
+        <v>42559</v>
       </c>
       <c r="L6" s="20">
         <f>IF(G6="","",G6+ROUND((IF(P7="",P6,P7)/(19*LN(IF(P7="",P6,P7))-42))*30,0))</f>
@@ -2238,11 +2246,11 @@
       </c>
       <c r="M6" s="20">
         <f>IF(K6="","",WORKDAY(K6,1))</f>
-        <v>42555</v>
+        <v>42562</v>
       </c>
       <c r="N6" s="20">
         <f>IF(M6="","",M6+SLA_PrazoGarantia)</f>
-        <v>42735</v>
+        <v>42742</v>
       </c>
       <c r="O6" s="29" t="str">
         <f>IF(A5="","","Previsto")</f>
@@ -2340,9 +2348,9 @@
         <f>IF(A5="","",IF(VLOOKUP(A5,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A5,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
         <v>42444</v>
       </c>
-      <c r="I7" s="20" t="str">
+      <c r="I7" s="20">
         <f>IF(A5="","",IF(VLOOKUP(A5,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A5,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42520</v>
       </c>
       <c r="J7" s="20" t="str">
         <f>IF(A5="","",IF(VLOOKUP(A5,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A5,OSS[],MATCH("Recebimento da OS",OSS[#Headers],0),FALSE)))</f>
@@ -2543,7 +2551,7 @@
       </c>
       <c r="B10" s="73" t="str">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Plano Entregue</v>
       </c>
       <c r="C10" s="73"/>
       <c r="D10" s="54" t="str">
@@ -2552,7 +2560,7 @@
       </c>
       <c r="E10" s="59">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42486</v>
+        <v>42500</v>
       </c>
       <c r="F10" s="68" t="str">
         <f>IF(A10="","","Titulo:")</f>
@@ -2735,9 +2743,9 @@
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
         <v>42493</v>
       </c>
-      <c r="H12" s="20" t="str">
+      <c r="H12" s="20">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42500</v>
       </c>
       <c r="I12" s="20" t="str">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Entrega da OS",OSS[#Headers],0),FALSE)))</f>
@@ -2942,7 +2950,7 @@
       </c>
       <c r="B15" s="73" t="str">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Iniciada</v>
       </c>
       <c r="C15" s="73"/>
       <c r="D15" s="54" t="str">
@@ -2951,7 +2959,7 @@
       </c>
       <c r="E15" s="59">
         <f>IF(A15="","",VLOOKUP(A15,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="F15" s="68" t="str">
         <f>IF(A15="","","Titulo:")</f>
@@ -3130,9 +3138,9 @@
         <v>94</v>
       </c>
       <c r="E17" s="37"/>
-      <c r="G17" s="20" t="str">
+      <c r="G17" s="20">
         <f>IF(A15="","",IF(VLOOKUP(A15,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A15,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42521</v>
       </c>
       <c r="H17" s="20" t="str">
         <f>IF(A15="","",IF(VLOOKUP(A15,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A15,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
@@ -3170,9 +3178,9 @@
         <f>IF(A15="","",IF(VLOOKUP(A15,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A15,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
         <v/>
       </c>
-      <c r="Q17" s="57" t="str">
-        <f>IF(F16="","",IF(G17="","",IF(L17="",IF(DataRef&lt;L16,L16,DataRef),L17)-L16))</f>
-        <v/>
+      <c r="Q17" s="57">
+        <f ca="1">IF(F16="","",IF(G17="","",IF(L17="",IF(DataRef&lt;L16,L16,DataRef),L17)-L16))</f>
+        <v>0</v>
       </c>
       <c r="R17" s="21" t="str">
         <f>IF(J17="","",AF16)</f>
@@ -3198,9 +3206,9 @@
         <f>IF(K17="","",AC17/IF($P17="",$P16,$P17))</f>
         <v/>
       </c>
-      <c r="X17" s="57" t="str">
-        <f ca="1">IF(F16="","",IF(G17="",IF(DataRef&lt;G16,"",DataRef-G16),G17-G16))</f>
-        <v/>
+      <c r="X17" s="57">
+        <f>IF(F16="","",IF(G17="",IF(DataRef&lt;G16,"",DataRef-G16),G17-G16))</f>
+        <v>0</v>
       </c>
       <c r="Y17" s="57" t="str">
         <f>IF(OR(R15="Hora Java",R15="Hora dotNet"),AG16,"")</f>
@@ -3262,7 +3270,7 @@
         <v/>
       </c>
       <c r="Q18" s="57" t="str">
-        <f>IF(Q17="","",IF(OR(Q16&gt;Q17,Z16&lt;Z17),"",ROUND(Q17*(IF($P17="",$P16,$P17)*SLA_ICA_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q17="","",IF(OR(Q16&gt;Q17,Z16&lt;Z17),"",ROUND(Q17*(IF($P17="",$P16,$P17)*SLA_ICA_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R18" s="57" t="str">
@@ -3290,7 +3298,7 @@
         <v/>
       </c>
       <c r="X18" s="57" t="str">
-        <f ca="1">IF(X17="","",IF(X16&gt;X17,"",ROUND(X17*(IF($P17="",$P16,$P17)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X17="","",IF(X16&gt;X17,"",ROUND(X17*(IF($P17="",$P16,$P17)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y18" s="57" t="str">
@@ -3341,7 +3349,7 @@
       </c>
       <c r="B20" s="73" t="str">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v>Aberta</v>
+        <v>Iniciada</v>
       </c>
       <c r="C20" s="73"/>
       <c r="D20" s="54" t="str">
@@ -3350,7 +3358,7 @@
       </c>
       <c r="E20" s="59">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="F20" s="68" t="str">
         <f>IF(A20="","","Titulo:")</f>
@@ -3419,27 +3427,27 @@
       </c>
       <c r="I21" s="20">
         <f>IF(G21="","",G21+ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30*SLA_PrazoEntrega,0))</f>
-        <v>42569</v>
+        <v>42571</v>
       </c>
       <c r="J21" s="20">
         <f>IF(I21="","",WORKDAY(I21,IF(IF(P22="",P21,P22)&lt;150,5,10)))</f>
-        <v>42576</v>
+        <v>42578</v>
       </c>
       <c r="K21" s="20">
         <f>IF(J21="","",J21+ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30*SLA_PrazoAceite,0))</f>
-        <v>42592</v>
+        <v>42595</v>
       </c>
       <c r="L21" s="20">
         <f>IF(G21="","",G21+ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30,0))</f>
-        <v>42600</v>
+        <v>42605</v>
       </c>
       <c r="M21" s="20">
         <f>IF(K21="","",WORKDAY(K21,1))</f>
-        <v>42593</v>
+        <v>42597</v>
       </c>
       <c r="N21" s="20">
         <f>IF(M21="","",M21+SLA_PrazoGarantia)</f>
-        <v>42773</v>
+        <v>42777</v>
       </c>
       <c r="O21" s="29" t="str">
         <f>IF(A20="","","Previsto")</f>
@@ -3447,11 +3455,11 @@
       </c>
       <c r="P21" s="21">
         <f>IF(A20="","",VLOOKUP(A20,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE))</f>
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="Q21" s="57">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICP_EOS,1))</f>
-        <v>7.9</v>
+        <v>8.4</v>
       </c>
       <c r="R21" s="21">
         <f>IF(F21="","",SLA_ICP_CIHA)</f>
@@ -3487,7 +3495,7 @@
       </c>
       <c r="Z21" s="57">
         <f>IF(F21="","",ROUND((L21-G21)*SLA_ICA_EOS,1))</f>
-        <v>19.8</v>
+        <v>21</v>
       </c>
       <c r="AA21" t="str">
         <f>IF(A20="","","Homologação")</f>
@@ -3526,12 +3534,12 @@
       <c r="C22" s="37"/>
       <c r="D22" s="37">
         <f ca="1">IF(P21="","",IF($P22="",$P21,$P22)+IF(P23="",0,P23)-IF(D21="",0,D21))</f>
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="E22" s="37"/>
-      <c r="G22" s="20" t="str">
+      <c r="G22" s="20">
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42521</v>
       </c>
       <c r="H22" s="20" t="str">
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
@@ -3569,9 +3577,9 @@
         <f>IF(A20="","",IF(VLOOKUP(A20,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A20,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
         <v/>
       </c>
-      <c r="Q22" s="57" t="str">
-        <f>IF(F21="","",IF(G22="","",IF(L22="",IF(DataRef&lt;L21,L21,DataRef),L22)-L21))</f>
-        <v/>
+      <c r="Q22" s="57">
+        <f ca="1">IF(F21="","",IF(G22="","",IF(L22="",IF(DataRef&lt;L21,L21,DataRef),L22)-L21))</f>
+        <v>0</v>
       </c>
       <c r="R22" s="21" t="str">
         <f>IF(J22="","",AF21)</f>
@@ -3597,9 +3605,9 @@
         <f>IF(K22="","",AC22/IF($P22="",$P21,$P22))</f>
         <v/>
       </c>
-      <c r="X22" s="57" t="str">
-        <f ca="1">IF(F21="","",IF(G22="",IF(DataRef&lt;G21,"",DataRef-G21),G22-G21))</f>
-        <v/>
+      <c r="X22" s="57">
+        <f>IF(F21="","",IF(G22="",IF(DataRef&lt;G21,"",DataRef-G21),G22-G21))</f>
+        <v>0</v>
       </c>
       <c r="Y22" s="57" t="str">
         <f>IF(OR(R20="Hora Java",R20="Hora dotNet"),AG21,"")</f>
@@ -3650,7 +3658,7 @@
       </c>
       <c r="L23" s="70">
         <f>IF(G21="","",ROUND((IF(P22="",P21,P22)/(19*LN(IF(P22="",P21,P22))-42))*30,0))</f>
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="O23" s="29" t="str">
         <f>IF(A20="","","Multa")</f>
@@ -3661,7 +3669,7 @@
         <v/>
       </c>
       <c r="Q23" s="57" t="str">
-        <f>IF(Q22="","",IF(OR(Q21&gt;Q22,Z21&lt;Z22),"",ROUND(Q22*(IF($P22="",$P21,$P22)*SLA_ICA_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q22="","",IF(OR(Q21&gt;Q22,Z21&lt;Z22),"",ROUND(Q22*(IF($P22="",$P21,$P22)*SLA_ICA_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R23" s="57" t="str">
@@ -3689,7 +3697,7 @@
         <v/>
       </c>
       <c r="X23" s="57" t="str">
-        <f ca="1">IF(X22="","",IF(X21&gt;X22,"",ROUND(X22*(IF($P22="",$P21,$P22)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X22="","",IF(X21&gt;X22,"",ROUND(X22*(IF($P22="",$P21,$P22)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y23" s="57" t="str">
@@ -14694,7 +14702,7 @@
       </c>
       <c r="H1" s="61" t="str">
         <f ca="1">YEAR(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1)&amp;TEXT(MONTH(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1),"00")</f>
-        <v>201604</v>
+        <v>201605</v>
       </c>
       <c r="I1" s="20"/>
       <c r="J1" t="s">
@@ -14702,21 +14710,21 @@
       </c>
       <c r="K1" s="20">
         <f ca="1">IF($L$1="",TODAY(),$L$1)</f>
-        <v>42495</v>
+        <v>42526</v>
       </c>
       <c r="L1" s="52">
         <f>IF(Mensal!B1="","",Mensal!B1)</f>
-        <v>42495</v>
+        <v>42526</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="str">
+      <c r="A2" s="21">
         <f t="shared" ref="A2:A15" ca="1" si="0">IF(E2=E1,"",E2)</f>
-        <v/>
-      </c>
-      <c r="B2" s="21" t="str">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21">
         <f ca="1">IF(C2="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C2,""))</f>
-        <v/>
+        <v>4721</v>
       </c>
       <c r="C2" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
@@ -14724,17 +14732,17 @@
       </c>
       <c r="D2" s="52">
         <f>IF(C2="","",VLOOKUP(C2,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42444</v>
-      </c>
-      <c r="E2" s="21" t="str">
+        <v>42520</v>
+      </c>
+      <c r="E2" s="21">
         <f t="shared" ref="E2:E15" ca="1" si="1">IF(B2="",E1,IF(E1="",1,E1)+1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="21">
         <f ca="1">IF(C3="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C3,""))</f>
@@ -14746,21 +14754,21 @@
       </c>
       <c r="D3" s="52">
         <f>IF(C3="","",VLOOKUP(C3,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42486</v>
+        <v>42500</v>
       </c>
       <c r="E3" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="str">
+      <c r="A4" s="21">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="B4" s="21" t="str">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21">
         <f ca="1">IF(C4="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C4,""))</f>
-        <v/>
+        <v>4776</v>
       </c>
       <c r="C4" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
@@ -14768,22 +14776,22 @@
       </c>
       <c r="D4" s="52">
         <f>IF(C4="","",VLOOKUP(C4,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="E4" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="str">
+      <c r="A5" s="21">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="B5" s="21" t="str">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21">
         <f ca="1">IF(C5="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C5,""))</f>
-        <v/>
+        <v>4777</v>
       </c>
       <c r="C5" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
@@ -14791,11 +14799,11 @@
       </c>
       <c r="D5" s="52">
         <f>IF(C5="","",VLOOKUP(C5,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v>42514</v>
+        <v>42521</v>
       </c>
       <c r="E5" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L5" s="21"/>
     </row>
@@ -14818,7 +14826,7 @@
       </c>
       <c r="E6" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L6" s="21"/>
     </row>
@@ -14841,7 +14849,7 @@
       </c>
       <c r="E7" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L7" s="21"/>
     </row>
@@ -14864,7 +14872,7 @@
       </c>
       <c r="E8" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L8" s="21"/>
     </row>
@@ -14887,7 +14895,7 @@
       </c>
       <c r="E9" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L9" s="21"/>
     </row>
@@ -14910,7 +14918,7 @@
       </c>
       <c r="E10" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L10" s="21"/>
     </row>
@@ -14933,7 +14941,7 @@
       </c>
       <c r="E11" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L11" s="21"/>
     </row>
@@ -14956,7 +14964,7 @@
       </c>
       <c r="E12" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -14978,7 +14986,7 @@
       </c>
       <c r="E13" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -15000,7 +15008,7 @@
       </c>
       <c r="E14" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -15022,7 +15030,7 @@
       </c>
       <c r="E15" s="21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -15044,7 +15052,7 @@
       </c>
       <c r="E16" s="21">
         <f t="shared" ref="E16:E30" ca="1" si="3">IF(B16="",E15,IF(E15="",1,E15)+1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -15066,7 +15074,7 @@
       </c>
       <c r="E17" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -15088,7 +15096,7 @@
       </c>
       <c r="E18" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -15110,7 +15118,7 @@
       </c>
       <c r="E19" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -15132,7 +15140,7 @@
       </c>
       <c r="E20" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -15154,7 +15162,7 @@
       </c>
       <c r="E21" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -15176,7 +15184,7 @@
       </c>
       <c r="E22" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -15198,7 +15206,7 @@
       </c>
       <c r="E23" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -15220,7 +15228,7 @@
       </c>
       <c r="E24" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -15242,7 +15250,7 @@
       </c>
       <c r="E25" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -15264,7 +15272,7 @@
       </c>
       <c r="E26" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -15286,7 +15294,7 @@
       </c>
       <c r="E27" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -15308,7 +15316,7 @@
       </c>
       <c r="E28" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -15330,7 +15338,7 @@
       </c>
       <c r="E29" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -15352,7 +15360,7 @@
       </c>
       <c r="E30" s="21">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -15374,7 +15382,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
OS 4782 - Produto Serviços Transversais - Subproduto Gestão de Segurança - Manter Funcionalidades e Perfil Versão (1.0).
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201606.xlsx
+++ b/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201606.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="145">
   <si>
     <t>Número OS</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Produto Serviços Transversais - Subproduto Gestão de Segurança - Manter Usuário Versão (1.0)</t>
+  </si>
+  <si>
+    <t>Produto Serviços Transversais - Subproduto Gestão de Segurança - Manter Funcionalidades e Perfil Versão (1.0)</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1311,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="OSS" displayName="OSS" ref="A1:V5" totalsRowShown="0" dataDxfId="25">
-  <autoFilter ref="A1:V5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="OSS" displayName="OSS" ref="A1:V6" totalsRowShown="0" dataDxfId="25">
+  <autoFilter ref="A1:V6"/>
   <sortState ref="A2:U15">
     <sortCondition ref="A1:A15"/>
   </sortState>
@@ -1682,13 +1685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,6 +1950,44 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
     </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>4782</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="52">
+        <v>42522</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="52">
+        <v>42522</v>
+      </c>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="21">
+        <v>153</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1967,7 +2008,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15:C15"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,30 +3783,30 @@
       <c r="P24" s="37"/>
     </row>
     <row r="25" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="str">
+      <c r="A25" s="54">
         <f>IF(ControleOSsMês!$G$1="Todas",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),""),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSMês[],2,FALSE),""))</f>
-        <v/>
+        <v>4782</v>
       </c>
       <c r="B25" s="73" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>Aberta</v>
       </c>
       <c r="C25" s="73"/>
       <c r="D25" s="54" t="str">
         <f>IF(A25="","","em")</f>
-        <v/>
-      </c>
-      <c r="E25" s="59" t="str">
+        <v>em</v>
+      </c>
+      <c r="E25" s="59">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>42522</v>
       </c>
       <c r="F25" s="68" t="str">
         <f>IF(A25="","","Titulo:")</f>
-        <v/>
+        <v>Titulo:</v>
       </c>
       <c r="G25" s="31" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Titulo",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>Produto Serviços Transversais - Subproduto Gestão de Segurança - Manter Funcionalidades e Perfil Versão (1.0)</v>
       </c>
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
@@ -3778,11 +3819,11 @@
       <c r="P25" s="30"/>
       <c r="Q25" s="68" t="str">
         <f>IF(A25="","","Tipo da OS:")</f>
-        <v/>
+        <v>Tipo da OS:</v>
       </c>
       <c r="R25" s="31" t="str">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Tipo",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>PF Java</v>
       </c>
       <c r="S25" s="30"/>
       <c r="T25" s="30"/>
@@ -3794,7 +3835,7 @@
       <c r="Z25" s="30"/>
       <c r="AA25" s="58" t="str">
         <f>IF(A25="","","Número de Inconformidades")</f>
-        <v/>
+        <v>Número de Inconformidades</v>
       </c>
       <c r="AB25" s="30"/>
       <c r="AC25" s="30"/>
@@ -3806,99 +3847,99 @@
     <row r="26" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="66" t="str">
         <f>IF(A25="","","PF Pago")</f>
-        <v/>
-      </c>
-      <c r="D26" t="str">
+        <v>PF Pago</v>
+      </c>
+      <c r="D26">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("PF Pago",OSS[#Headers],0),FALSE))</f>
-        <v/>
-      </c>
-      <c r="F26" s="36" t="str">
+        <v>0</v>
+      </c>
+      <c r="F26" s="36">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("Abertura da OS",OSS[#Headers],0),FALSE))</f>
-        <v/>
-      </c>
-      <c r="G26" s="20" t="str">
+        <v>42522</v>
+      </c>
+      <c r="G26" s="20">
         <f>IF(F26="","",WORKDAY(F26,IF(IF(P27="",P26,P27)&lt;150,5,10)))</f>
-        <v/>
-      </c>
-      <c r="H26" s="20" t="str">
+        <v>42536</v>
+      </c>
+      <c r="H26" s="20">
         <f>IF(G26="","",WORKDAY(G26,5))</f>
-        <v/>
-      </c>
-      <c r="I26" s="20" t="str">
+        <v>42543</v>
+      </c>
+      <c r="I26" s="20">
         <f>IF(G26="","",G26+ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30*SLA_PrazoEntrega,0))</f>
-        <v/>
-      </c>
-      <c r="J26" s="20" t="str">
+        <v>42587</v>
+      </c>
+      <c r="J26" s="20">
         <f>IF(I26="","",WORKDAY(I26,IF(IF(P27="",P26,P27)&lt;150,5,10)))</f>
-        <v/>
-      </c>
-      <c r="K26" s="20" t="str">
+        <v>42601</v>
+      </c>
+      <c r="K26" s="20">
         <f>IF(J26="","",J26+ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30*SLA_PrazoAceite,0))</f>
-        <v/>
-      </c>
-      <c r="L26" s="20" t="str">
+        <v>42618</v>
+      </c>
+      <c r="L26" s="20">
         <f>IF(G26="","",G26+ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30,0))</f>
-        <v/>
-      </c>
-      <c r="M26" s="20" t="str">
+        <v>42622</v>
+      </c>
+      <c r="M26" s="20">
         <f>IF(K26="","",WORKDAY(K26,1))</f>
-        <v/>
-      </c>
-      <c r="N26" s="20" t="str">
+        <v>42619</v>
+      </c>
+      <c r="N26" s="20">
         <f>IF(M26="","",M26+SLA_PrazoGarantia)</f>
-        <v/>
+        <v>42799</v>
       </c>
       <c r="O26" s="29" t="str">
         <f>IF(A25="","","Previsto")</f>
-        <v/>
-      </c>
-      <c r="P26" s="21" t="str">
+        <v>Previsto</v>
+      </c>
+      <c r="P26" s="21">
         <f>IF(A25="","",VLOOKUP(A25,OSS[],MATCH("PF Previsto",OSS[#Headers],0),FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q26" s="57" t="str">
+        <v>153</v>
+      </c>
+      <c r="Q26" s="57">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICP_EOS,1))</f>
-        <v/>
-      </c>
-      <c r="R26" s="21" t="str">
+        <v>8.6</v>
+      </c>
+      <c r="R26" s="21">
         <f>IF(F26="","",SLA_ICP_CIHA)</f>
-        <v/>
-      </c>
-      <c r="S26" s="21" t="str">
+        <v>2</v>
+      </c>
+      <c r="S26" s="21">
         <f>IF(F26="","",SLA_ICP_CIG)</f>
-        <v/>
-      </c>
-      <c r="T26" s="57" t="str">
+        <v>2</v>
+      </c>
+      <c r="T26" s="57">
         <f>IF(F26="","",SLA_IQA_INGHA)</f>
-        <v/>
-      </c>
-      <c r="U26" s="57" t="str">
+        <v>0.2</v>
+      </c>
+      <c r="U26" s="57">
         <f>IF(F26="","",SLA_IQA_IGHA)</f>
-        <v/>
-      </c>
-      <c r="V26" s="57" t="str">
+        <v>0.05</v>
+      </c>
+      <c r="V26" s="57">
         <f>IF(F26="","",SLA_IQA_INGG)</f>
-        <v/>
-      </c>
-      <c r="W26" s="57" t="str">
+        <v>0.05</v>
+      </c>
+      <c r="W26" s="57">
         <f>IF(F26="","",SLA_IQA_IGG)</f>
-        <v/>
-      </c>
-      <c r="X26" s="57" t="str">
+        <v>0.01</v>
+      </c>
+      <c r="X26" s="57">
         <f>IF(F26="","",ROUND((G26-F26)*SLA_ICA_IOS,1))</f>
-        <v/>
+        <v>1.4</v>
       </c>
       <c r="Y26" s="57" t="str">
         <f>IF(OR(R25="Hora Java",R25="Hora dotNet"),SLA_ICA_SP,"")</f>
         <v/>
       </c>
-      <c r="Z26" s="57" t="str">
+      <c r="Z26" s="57">
         <f>IF(F26="","",ROUND((L26-G26)*SLA_ICA_EOS,1))</f>
-        <v/>
+        <v>21.5</v>
       </c>
       <c r="AA26" t="str">
         <f>IF(A25="","","Homologação")</f>
-        <v/>
+        <v>Homologação</v>
       </c>
       <c r="AB26" s="21" t="str">
         <f>IF(J27="","",VLOOKUP(A25,OSS[],MATCH("Não Grave - Homologação",OSS[#Headers],0),FALSE))</f>
@@ -3928,12 +3969,12 @@
     <row r="27" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="66" t="str">
         <f>IF(A25="","","Saldo de PF")</f>
-        <v/>
+        <v>Saldo de PF</v>
       </c>
       <c r="C27" s="37"/>
-      <c r="D27" s="37" t="str">
-        <f>IF(P26="","",IF($P27="",$P26,$P27)+IF(P28="",0,P28)-IF(D26="",0,D26))</f>
-        <v/>
+      <c r="D27" s="37">
+        <f ca="1">IF(P26="","",IF($P27="",$P26,$P27)+IF(P28="",0,P28)-IF(D26="",0,D26))</f>
+        <v>153</v>
       </c>
       <c r="E27" s="37"/>
       <c r="G27" s="20" t="str">
@@ -3970,7 +4011,7 @@
       </c>
       <c r="O27" s="29" t="str">
         <f>IF(A25="","","Apurado")</f>
-        <v/>
+        <v>Apurado</v>
       </c>
       <c r="P27" s="21" t="str">
         <f>IF(A25="","",IF(VLOOKUP(A25,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A25,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
@@ -4005,20 +4046,20 @@
         <v/>
       </c>
       <c r="X27" s="57" t="str">
-        <f>IF(F26="","",IF(G27="",IF(DataRef&lt;G26,"",DataRef-G26),G27-G26))</f>
+        <f ca="1">IF(F26="","",IF(G27="",IF(DataRef&lt;G26,"",DataRef-G26),G27-G26))</f>
         <v/>
       </c>
       <c r="Y27" s="57" t="str">
         <f>IF(OR(R25="Hora Java",R25="Hora dotNet"),AG26,"")</f>
         <v/>
       </c>
-      <c r="Z27" s="57" t="str">
-        <f>IF(F26="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26)</f>
-        <v/>
+      <c r="Z27" s="57">
+        <f ca="1">IF(F26="","",IF(L27="",IF(DataRef&lt;L26,L26,DataRef),L27)-L26)</f>
+        <v>0</v>
       </c>
       <c r="AA27" t="str">
         <f>IF(A25="","","Garantia")</f>
-        <v/>
+        <v>Garantia</v>
       </c>
       <c r="AB27" s="21" t="str">
         <f>IF(K27="","",VLOOKUP(A25,OSS[],MATCH("Não Grave - Garantia",OSS[#Headers],0),FALSE))</f>
@@ -4044,27 +4085,27 @@
     <row r="28" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="66" t="str">
         <f>IF(A25="","","PF a Pagar")</f>
-        <v/>
-      </c>
-      <c r="C28" s="67" t="str">
-        <f>IF(D27="","",IF(B25="Recebida",(P27*0.8),IF(B25="Aceita",D27,0))+IF(D27&lt;0,D27,0))</f>
-        <v/>
+        <v>PF a Pagar</v>
+      </c>
+      <c r="C28" s="67">
+        <f ca="1">IF(D27="","",IF(B25="Recebida",(P27*0.8),IF(B25="Aceita",D27,0))+IF(D27&lt;0,D27,0))</f>
+        <v>0</v>
       </c>
       <c r="E28" s="37"/>
       <c r="K28" s="69" t="str">
         <f>IF(A25="","","Prazo previsto para execução em dias corridos")</f>
-        <v/>
-      </c>
-      <c r="L28" s="70" t="str">
+        <v>Prazo previsto para execução em dias corridos</v>
+      </c>
+      <c r="L28" s="70">
         <f>IF(G26="","",ROUND((IF(P27="",P26,P27)/(19*LN(IF(P27="",P26,P27))-42))*30,0))</f>
-        <v/>
+        <v>86</v>
       </c>
       <c r="O28" s="29" t="str">
         <f>IF(A25="","","Multa")</f>
-        <v/>
+        <v>Multa</v>
       </c>
       <c r="P28" s="25" t="str">
-        <f>IF(SUM(Q28:Z28)=0,"",-ROUND(SUM(Q28:Z28),0))</f>
+        <f ca="1">IF(SUM(Q28:Z28)=0,"",-ROUND(SUM(Q28:Z28),0))</f>
         <v/>
       </c>
       <c r="Q28" s="57" t="str">
@@ -4096,7 +4137,7 @@
         <v/>
       </c>
       <c r="X28" s="57" t="str">
-        <f>IF(X27="","",IF(X26&gt;X27,"",ROUND(X27*(IF($P27="",$P26,$P27)*SLA_ICA_IOS_Multa),2)))</f>
+        <f ca="1">IF(X27="","",IF(X26&gt;X27,"",ROUND(X27*(IF($P27="",$P26,$P27)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y28" s="57" t="str">
@@ -4104,12 +4145,12 @@
         <v/>
       </c>
       <c r="Z28" s="57" t="str">
-        <f>IF(Z27="","",IF(Z26&gt;Z27,"",ROUND(IF($P27="",$P26,$P27)*SLA_ICA_EOS_Multa,2)))</f>
+        <f ca="1">IF(Z27="","",IF(Z26&gt;Z27,"",ROUND(IF($P27="",$P26,$P27)*SLA_ICA_EOS_Multa,2)))</f>
         <v/>
       </c>
       <c r="AA28" t="str">
         <f>IF(A25="","","Total")</f>
-        <v/>
+        <v>Total</v>
       </c>
       <c r="AB28" s="21" t="str">
         <f>IF(SUM(AB26:AB27)=0,"",SUM(AB26:AB27))</f>
@@ -14117,6 +14158,25 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B110:C110"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:C5"/>
@@ -14129,25 +14189,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B145:C145"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -14813,16 +14854,16 @@
         <v/>
       </c>
       <c r="B6" s="21" t="str">
-        <f>IF(C6="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C6,""))</f>
-        <v/>
-      </c>
-      <c r="C6" s="21" t="str">
+        <f ca="1">IF(C6="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C6,""))</f>
+        <v/>
+      </c>
+      <c r="C6" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
-        <v/>
-      </c>
-      <c r="D6" s="52" t="str">
+        <v>4782</v>
+      </c>
+      <c r="D6" s="52">
         <f>IF(C6="","",VLOOKUP(C6,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
-        <v/>
+        <v>42522</v>
       </c>
       <c r="E6" s="21">
         <f t="shared" ca="1" si="1"/>
@@ -15382,7 +15423,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>